<commit_message>
Merged PR 1435: Added input-definition and script logic for creating virtual directories.
Added input-definition and script logic for creating virtual directories.

Related work items: #30633
</commit_message>
<xml_diff>
--- a/DevOps/Server Setup/IIS/IIS Web App Setup Definitions For TSV Export.xlsx
+++ b/DevOps/Server Setup/IIS/IIS Web App Setup Definitions For TSV Export.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\irmaqafile\e$\IRMA\Staging\docs\Projects\IIS Web App Setup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tlux\dev\git\Icon\DevOps\Server Setup\IIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Test App Pools" sheetId="3" r:id="rId3"/>
     <sheet name="Web Apps" sheetId="2" r:id="rId4"/>
     <sheet name="Legacy Apps" sheetId="4" r:id="rId5"/>
+    <sheet name="Virtual Directories" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="66">
   <si>
     <t>IISAppPoolName</t>
   </si>
@@ -178,9 +179,6 @@
   </si>
   <si>
     <t>SPOReportsDev</t>
-  </si>
-  <si>
-    <t>SPOReport</t>
   </si>
   <si>
     <t>WFM\SPOReportsDev</t>
@@ -221,6 +219,15 @@
   </si>
   <si>
     <t>enable32BitAppOnWin64=True</t>
+  </si>
+  <si>
+    <t>vName</t>
+  </si>
+  <si>
+    <t>sporefiles</t>
+  </si>
+  <si>
+    <t>E:\WebTools\PO\</t>
   </si>
 </sst>
 </file>
@@ -710,7 +717,7 @@
         <v>20</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -766,16 +773,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5" t="s">
         <v>34</v>
@@ -783,7 +790,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -817,7 +824,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -834,7 +841,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -863,7 +870,7 @@
         <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -967,7 +974,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,7 +1015,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -1050,13 +1057,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
         <v>32</v>
@@ -1078,30 +1085,30 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
         <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
         <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1120,16 +1127,16 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
         <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1255,4 +1262,46 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="35.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Merged PR 94: New Dev Server Env Full Rerun
- Added 'new-folder' option in Security input script and option to return and skip perms setup (so it just creates folder); needed for SPORe.  Added regional web-app input defs.
- Added common Functions PS script.  Fixed mismatch between RM and SO in web app def TSV.  Updated Security-Setup script: script folder assumed for input files, preview mode option, output and stop after each section.  Standardized main Security and IIS setup scripts to determine its own script folder, load functions script, create transcript log, and prompt for preview mode.

Related work items: #4399
</commit_message>
<xml_diff>
--- a/DevOps/Server Setup/IIS/IIS Web App Setup Definitions For TSV Export.xlsx
+++ b/DevOps/Server Setup/IIS/IIS Web App Setup Definitions For TSV Export.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tlux\dev\git\Icon\DevOps\Server Setup\IIS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tlux\dev\git\scad\DevOps\Server Setup\IIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15660" windowHeight="6765" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15660" windowHeight="6765" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="IGNORE" sheetId="1" r:id="rId1"/>
     <sheet name="Dev App Pools" sheetId="5" r:id="rId2"/>
-    <sheet name="Test App Pools" sheetId="3" r:id="rId3"/>
-    <sheet name="Web Apps" sheetId="2" r:id="rId4"/>
-    <sheet name="Legacy Apps" sheetId="4" r:id="rId5"/>
-    <sheet name="Virtual Directories" sheetId="7" r:id="rId6"/>
+    <sheet name="Web Apps" sheetId="2" r:id="rId3"/>
+    <sheet name="Legacy Apps" sheetId="4" r:id="rId4"/>
+    <sheet name="Virtual Directories" sheetId="7" r:id="rId5"/>
+    <sheet name="Test App Pools" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="81">
   <si>
     <t>IISAppPoolName</t>
   </si>
@@ -228,6 +228,51 @@
   </si>
   <si>
     <t>E:\WebTools\PO\</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>SO</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>XX</t>
+  </si>
+  <si>
+    <t>IRMAWebMWDev</t>
+  </si>
+  <si>
+    <t>IRMAWebSODev</t>
+  </si>
+  <si>
+    <t>IRMAWebRMDev</t>
+  </si>
+  <si>
+    <t>IRMAWebUKDev</t>
+  </si>
+  <si>
+    <t>IRMAWebXXDev</t>
+  </si>
+  <si>
+    <t>E:\Regions\FL\</t>
+  </si>
+  <si>
+    <t>E:\Regions\MW\</t>
+  </si>
+  <si>
+    <t>E:\Regions\SO\</t>
+  </si>
+  <si>
+    <t>E:\Regions\UK\</t>
+  </si>
+  <si>
+    <t>fz4VVLE9</t>
+  </si>
+  <si>
+    <t>WFM\IconWebTest</t>
   </si>
 </sst>
 </file>
@@ -689,10 +734,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E15" sqref="A2:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,7 +852,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -824,7 +869,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -841,7 +886,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -853,12 +898,12 @@
         <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -870,7 +915,92 @@
         <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -881,99 +1011,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="4" width="24.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
-  <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -1071,72 +1111,142 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1145,12 +1255,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A2" sqref="A2:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,10 +1332,10 @@
         <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
         <v>38</v>
@@ -1236,10 +1346,10 @@
         <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="D6" t="s">
         <v>40</v>
@@ -1250,12 +1360,180 @@
         <v>41</v>
       </c>
       <c r="B7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>28</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1264,7 +1542,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1304,4 +1582,102 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="4" width="24.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>